<commit_message>
Assessment artifacts Juan Antonio Cordoba R.
</commit_message>
<xml_diff>
--- a/Assessment/TestCases_Computer_Database.xlsx
+++ b/Assessment/TestCases_Computer_Database.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\Python\Code\Assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EA639C-A69B-4619-845C-E07D79BEAD83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF28CCE8-21E2-4CAE-940B-7EECFF972EF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-1965" windowWidth="19440" windowHeight="15000" xr2:uid="{4BE0AE26-F41D-43F2-B452-6E3580CBB6B2}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="63">
   <si>
     <t>Title</t>
   </si>
@@ -357,6 +357,11 @@
   </si>
   <si>
     <t>#</t>
+  </si>
+  <si>
+    <t>"""
+Created by Juan Antonio Cordoba
+"""</t>
   </si>
 </sst>
 </file>
@@ -498,17 +503,17 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="medium">
           <color indexed="64"/>
         </top>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -583,11 +588,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{52BF69B9-6AC8-45F5-91E9-3DFAE2D5B6CF}" name="Tabla3" displayName="Tabla3" ref="A16:B24" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{52BF69B9-6AC8-45F5-91E9-3DFAE2D5B6CF}" name="Tabla3" displayName="Tabla3" ref="A16:B24" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" tableBorderDxfId="2">
   <autoFilter ref="A16:B24" xr:uid="{944E5220-9522-4623-A615-7F782CA0C7A0}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C605BEC5-56DB-4A77-ACD4-34EC1575BD34}" name="#" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{129C6978-B7B5-4304-A788-03D0BB5C44CC}" name="Functionality" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{C605BEC5-56DB-4A77-ACD4-34EC1575BD34}" name="#" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{129C6978-B7B5-4304-A788-03D0BB5C44CC}" name="Functionality" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -904,8 +909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF4BB193-7089-45E3-AF8D-5CA3AD431C25}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,11 +1235,14 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>51</v>
       </c>
       <c r="B15" s="6"/>
+      <c r="E15" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">

</xml_diff>